<commit_message>
updating psi, xi ecs section 5.5
</commit_message>
<xml_diff>
--- a/TestEstandar.xlsx
+++ b/TestEstandar.xlsx
@@ -486,10 +486,10 @@
         <v>29.0926</v>
       </c>
       <c r="E2" t="n">
-        <v>828</v>
+        <v>853</v>
       </c>
       <c r="F2" t="n">
-        <v>151</v>
+        <v>176</v>
       </c>
       <c r="G2" t="n">
         <v>613</v>
@@ -514,10 +514,10 @@
         <v>15.1861</v>
       </c>
       <c r="E3" t="n">
-        <v>410</v>
+        <v>435</v>
       </c>
       <c r="F3" t="n">
-        <v>-20</v>
+        <v>5</v>
       </c>
       <c r="G3" t="n">
         <v>323</v>
@@ -542,10 +542,10 @@
         <v>15.208</v>
       </c>
       <c r="E4" t="n">
-        <v>282</v>
+        <v>307</v>
       </c>
       <c r="F4" t="n">
-        <v>296</v>
+        <v>321</v>
       </c>
       <c r="G4" t="n">
         <v>327</v>
@@ -570,10 +570,10 @@
         <v>28.0871</v>
       </c>
       <c r="E5" t="n">
-        <v>652</v>
+        <v>677</v>
       </c>
       <c r="F5" t="n">
-        <v>481</v>
+        <v>506</v>
       </c>
       <c r="G5" t="n">
         <v>593</v>

</xml_diff>

<commit_message>
adding heuristica avg error x,y
</commit_message>
<xml_diff>
--- a/TestEstandar.xlsx
+++ b/TestEstandar.xlsx
@@ -486,10 +486,10 @@
         <v>29.0926</v>
       </c>
       <c r="E2" t="n">
-        <v>828</v>
+        <v>806.5705</v>
       </c>
       <c r="F2" t="n">
-        <v>-184</v>
+        <v>318.68575</v>
       </c>
       <c r="G2" t="n">
         <v>613</v>
@@ -514,10 +514,10 @@
         <v>15.1861</v>
       </c>
       <c r="E3" t="n">
-        <v>410</v>
+        <v>388.5705</v>
       </c>
       <c r="F3" t="n">
-        <v>-186</v>
+        <v>489.68575</v>
       </c>
       <c r="G3" t="n">
         <v>323</v>
@@ -542,10 +542,10 @@
         <v>15.208</v>
       </c>
       <c r="E4" t="n">
-        <v>282</v>
+        <v>260.5705</v>
       </c>
       <c r="F4" t="n">
-        <v>182</v>
+        <v>173.68575</v>
       </c>
       <c r="G4" t="n">
         <v>327</v>
@@ -570,10 +570,10 @@
         <v>28.0871</v>
       </c>
       <c r="E5" t="n">
-        <v>652</v>
+        <v>630.5705</v>
       </c>
       <c r="F5" t="n">
-        <v>217</v>
+        <v>11.31425000000002</v>
       </c>
       <c r="G5" t="n">
         <v>593</v>

</xml_diff>

<commit_message>
using linear interpolator and avg error
</commit_message>
<xml_diff>
--- a/TestEstandar.xlsx
+++ b/TestEstandar.xlsx
@@ -486,10 +486,10 @@
         <v>29.0926</v>
       </c>
       <c r="E2" t="n">
-        <v>806.5705</v>
+        <v>792.927</v>
       </c>
       <c r="F2" t="n">
-        <v>318.68575</v>
+        <v>-70.439016520271</v>
       </c>
       <c r="G2" t="n">
         <v>613</v>
@@ -514,10 +514,10 @@
         <v>15.1861</v>
       </c>
       <c r="E3" t="n">
-        <v>388.5705</v>
+        <v>383.065</v>
       </c>
       <c r="F3" t="n">
-        <v>489.68575</v>
+        <v>1018.382359662934</v>
       </c>
       <c r="G3" t="n">
         <v>323</v>
@@ -542,10 +542,10 @@
         <v>15.208</v>
       </c>
       <c r="E4" t="n">
-        <v>260.5705</v>
+        <v>268.239</v>
       </c>
       <c r="F4" t="n">
-        <v>173.68575</v>
+        <v>16226.40414747018</v>
       </c>
       <c r="G4" t="n">
         <v>327</v>
@@ -570,10 +570,10 @@
         <v>28.0871</v>
       </c>
       <c r="E5" t="n">
-        <v>630.5705</v>
+        <v>642.051</v>
       </c>
       <c r="F5" t="n">
-        <v>11.31425000000002</v>
+        <v>-82696.38293800216</v>
       </c>
       <c r="G5" t="n">
         <v>593</v>

</xml_diff>